<commit_message>
Add index entry abt JMeter and JVM tunning, Add Fundadores entry on jtopen
</commit_message>
<xml_diff>
--- a/fundadores_project.xlsx
+++ b/fundadores_project.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>一個簡單的接口, hasMoreElement和nextElement, 在Properties看到有所應用, 當要遍歷HashTable時, 將h,key()賦給一個臨時的Enumeration 類(這key大有文章, 是由HashTable中的inner class Enumerator 實現的), 再以for 的三段式利用hasMoreElement()和nextElement()來Iterate</t>
   </si>
@@ -67,13 +67,49 @@
   </si>
   <si>
     <t>Detail</t>
+  </si>
+  <si>
+    <t>It is fun, like music, like literature, like art</t>
+  </si>
+  <si>
+    <t>the beauty in mathematic</t>
+  </si>
+  <si>
+    <t>the art of code, the message between lines</t>
+  </si>
+  <si>
+    <t>Jtopen</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Use Eclipse to read code</t>
+  </si>
+  <si>
+    <t>&lt;detail refers to index.xlsx where I note how to setup maven source sync env in eclipse&gt;</t>
+  </si>
+  <si>
+    <t>com.ibm.as400.access.AS400
+com.ibm.as400.access.ProgramParameter
+com.ibm.as400.access.ProgramCall</t>
+  </si>
+  <si>
+    <t>* Learn that jtopen is more flat in terms of structure
+* it used sync/ transient a lot
+* its private member is named like name_
+* programparameter's core is byte[] for input / output data, and int for length
+* In AS400 class, it use signon(args…) to form a routing of the same method
+    signon()  &gt; signon(Sting, String) &gt; signon(String, String, Credit)...
+* The signon behind AS400 is performed by AS400Impl interface, and this interface is implemented by AS400ImplProxy and AS400ImplRemote. 
+* Above interface and implementation relations is common in jtopen like the core behind ProgramCall : RemoteCommandImpl and its implementers Proxy and Remote</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +129,13 @@
       <name val="Calibri"/>
       <family val="3"/>
       <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -122,7 +165,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -130,7 +173,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -432,20 +476,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" customWidth="1"/>
-    <col min="3" max="3" width="84" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="43.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="70.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="41" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -456,59 +501,90 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="60">
-      <c r="A3" t="s">
+    <row r="2" spans="1:4" ht="45.75">
+      <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="B3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="45">
-      <c r="A5" t="s">
+      <c r="D3" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="34.5">
+      <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
+      <c r="D4" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="45">
-      <c r="A7" t="s">
+    <row r="6" spans="1:4" ht="23.25">
+      <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="B6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="B7" s="3" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>7</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="113.25">
+      <c r="A8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>